<commit_message>
Updated the cam file for jlcpcb. The other files are just minor changes
idk bro seems pretty sketchy
</commit_message>
<xml_diff>
--- a/v01partnumbers__digikey.xlsx
+++ b/v01partnumbers__digikey.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schandi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schandi\Documents\Projekte\WordClock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CFC30B0A-5837-4CAC-B0D2-D4AFB6B72EB7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8B02356B-C531-4523-A6EB-559B563BCB4D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12816" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -553,20 +553,20 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="6.42578125" customWidth="1"/>
+    <col min="1" max="2" width="6.44140625" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" customWidth="1"/>
-    <col min="5" max="5" width="40.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="28.5546875" customWidth="1"/>
+    <col min="5" max="5" width="40.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="20.88671875" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" customWidth="1"/>
+    <col min="10" max="10" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">

</xml_diff>